<commit_message>
Update of GINF3 Modules
</commit_message>
<xml_diff>
--- a/resources/GINF3/modules.xlsx
+++ b/resources/GINF3/modules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\AP1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55EF1FE-CDD7-4DCC-82C2-D60955CDB4C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06256FE7-ACDB-459D-9864-2C83F2BC9D1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="2760" windowWidth="15375" windowHeight="8325" xr2:uid="{4C56605D-1814-484D-BD67-6BFC85BD123D}"/>
+    <workbookView xWindow="5880" yWindow="3225" windowWidth="15375" windowHeight="8325" xr2:uid="{4C56605D-1814-484D-BD67-6BFC85BD123D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Code</t>
   </si>
@@ -37,6 +37,75 @@
   </si>
   <si>
     <t>Chef  Module</t>
+  </si>
+  <si>
+    <t>GINF1</t>
+  </si>
+  <si>
+    <t>GINF52</t>
+  </si>
+  <si>
+    <t>GINF53</t>
+  </si>
+  <si>
+    <t>GINF54</t>
+  </si>
+  <si>
+    <t>GINF55</t>
+  </si>
+  <si>
+    <t>GINF56</t>
+  </si>
+  <si>
+    <t>Technologies Net et J2EE</t>
+  </si>
+  <si>
+    <t>IA Avancée et Ingénierie de connaissance</t>
+  </si>
+  <si>
+    <t>Systèmes d'information et BI</t>
+  </si>
+  <si>
+    <t>Management des SI</t>
+  </si>
+  <si>
+    <t>Web Services et applications</t>
+  </si>
+  <si>
+    <t>Management de l'entreprise</t>
+  </si>
+  <si>
+    <t>El Haddad</t>
+  </si>
+  <si>
+    <t>El Alami Hassoun</t>
+  </si>
+  <si>
+    <t>Badir</t>
+  </si>
+  <si>
+    <t>Ezzine</t>
+  </si>
+  <si>
+    <t>Ben Achhab</t>
+  </si>
+  <si>
+    <t>Architecture J2EE, Prog Mobile Net</t>
+  </si>
+  <si>
+    <t>Datawarehouse, Dtatamining, BigData et Applications</t>
+  </si>
+  <si>
+    <t>Gouvernance des SI, ERP &amp; CRM, Audit &amp; Sécurité des SI</t>
+  </si>
+  <si>
+    <t>IA Avancée &amp; Web Sémantique, Ingénierie de connaissances</t>
+  </si>
+  <si>
+    <t>Dév Web en .net, Webservices, E-commerce et applications</t>
+  </si>
+  <si>
+    <t>Création d'Entreprise, Projets libres, Simulation d'entretien d'embauche et éthique de l'ingénieur</t>
   </si>
 </sst>
 </file>
@@ -388,16 +457,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9078595-6E23-491B-9A56-4D7BC37B86BD}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -414,6 +484,90 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>